<commit_message>
Restored files from commit 2236d1f...
</commit_message>
<xml_diff>
--- a/backtest_results.xlsx
+++ b/backtest_results.xlsx
@@ -435,10 +435,10 @@
         <v>1000</v>
       </c>
       <c r="D2">
-        <v>1195.945607539529</v>
+        <v>989.1059061551631</v>
       </c>
       <c r="E2">
-        <v>19.59456075395292</v>
+        <v>-1.089409384483686</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -452,10 +452,10 @@
         <v>1000</v>
       </c>
       <c r="D3">
-        <v>1155.883248478132</v>
+        <v>980.279774071637</v>
       </c>
       <c r="E3">
-        <v>15.58832484781318</v>
+        <v>-1.972022592836298</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -486,10 +486,10 @@
         <v>1000</v>
       </c>
       <c r="D5">
-        <v>1026.040042387351</v>
+        <v>998.1188647823619</v>
       </c>
       <c r="E5">
-        <v>2.604004238735125</v>
+        <v>-0.1881135217638108</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -503,10 +503,10 @@
         <v>1000</v>
       </c>
       <c r="D6">
-        <v>1083.738679021367</v>
+        <v>998.1188647823619</v>
       </c>
       <c r="E6">
-        <v>8.373867902136666</v>
+        <v>-0.1881135217638108</v>
       </c>
     </row>
     <row r="7" spans="1:5">

</xml_diff>

<commit_message>
Added regression and figured the samples, time steps, features part of LSTM to an extent
</commit_message>
<xml_diff>
--- a/backtest_results.xlsx
+++ b/backtest_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
   <si>
     <t>Stock Ticker</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Algorithm</t>
   </si>
   <si>
+    <t>methodology</t>
+  </si>
+  <si>
     <t>Initial Balance</t>
   </si>
   <si>
@@ -44,6 +47,12 @@
   </si>
   <si>
     <t>VWAP</t>
+  </si>
+  <si>
+    <t>classification</t>
+  </si>
+  <si>
+    <t>regression</t>
   </si>
 </sst>
 </file>
@@ -401,13 +410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,107 +432,202 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>1000</v>
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>989.1059061551631</v>
+        <v>1000</v>
       </c>
       <c r="E2">
-        <v>-1.089409384483686</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>985.8895705521473</v>
+      </c>
+      <c r="F2">
+        <v>-1.411042944785268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <v>896.7208884810494</v>
+      </c>
+      <c r="F3">
+        <v>-10.32791115189505</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>1000</v>
-      </c>
-      <c r="D3">
-        <v>980.279774071637</v>
-      </c>
-      <c r="E3">
-        <v>-1.972022592836298</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>1000</v>
+      <c r="C4" t="s">
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>1057.389974846661</v>
+        <v>1000</v>
       </c>
       <c r="E4">
-        <v>5.738997484666084</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>894.8501091417539</v>
+      </c>
+      <c r="F4">
+        <v>-10.51498908582461</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>1000</v>
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
       <c r="D5">
-        <v>998.1188647823619</v>
+        <v>1000</v>
       </c>
       <c r="E5">
-        <v>-0.1881135217638108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>1001.870779339296</v>
+      </c>
+      <c r="F5">
+        <v>0.1870779339295581</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>1000</v>
+      </c>
+      <c r="E6">
+        <v>1000.570825680124</v>
+      </c>
+      <c r="F6">
+        <v>0.05708256801236758</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
-        <v>1000</v>
-      </c>
-      <c r="D6">
-        <v>998.1188647823619</v>
-      </c>
-      <c r="E6">
-        <v>-0.1881135217638108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>1000</v>
+      </c>
+      <c r="E7">
+        <v>1016.698409886167</v>
+      </c>
+      <c r="F7">
+        <v>1.669840988616733</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C7">
-        <v>1000</v>
-      </c>
-      <c r="D7">
-        <v>1227.209074236686</v>
-      </c>
-      <c r="E7">
-        <v>22.72090742366856</v>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>1000</v>
+      </c>
+      <c r="E8">
+        <v>1016.698409886167</v>
+      </c>
+      <c r="F8">
+        <v>1.669840988616733</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>1000</v>
+      </c>
+      <c r="E9">
+        <v>991.3163165158546</v>
+      </c>
+      <c r="F9">
+        <v>-0.8683683484145388</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>1000</v>
+      </c>
+      <c r="E10">
+        <v>1000</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>1000</v>
+      </c>
+      <c r="E11">
+        <v>1124.453764535177</v>
+      </c>
+      <c r="F11">
+        <v>12.4453764535177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backing up the most current
</commit_message>
<xml_diff>
--- a/backtest_results.xlsx
+++ b/backtest_results.xlsx
@@ -450,10 +450,10 @@
         <v>1000</v>
       </c>
       <c r="E2">
-        <v>990.5413814561294</v>
+        <v>1306.472775194389</v>
       </c>
       <c r="F2">
-        <v>-0.9458618543870534</v>
+        <v>30.64727751943894</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -470,10 +470,10 @@
         <v>1000</v>
       </c>
       <c r="E3">
-        <v>896.7208884810494</v>
+        <v>773.9697588173583</v>
       </c>
       <c r="F3">
-        <v>-10.32791115189505</v>
+        <v>-22.60302411826417</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -490,10 +490,10 @@
         <v>1000</v>
       </c>
       <c r="E4">
-        <v>890.4766276913342</v>
+        <v>-2029.447346335359</v>
       </c>
       <c r="F4">
-        <v>-10.95233723086658</v>
+        <v>-302.9447346335359</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -510,10 +510,10 @@
         <v>1000</v>
       </c>
       <c r="E5">
-        <v>888.6058483520386</v>
+        <v>1581.975128548893</v>
       </c>
       <c r="F5">
-        <v>-11.13941516479614</v>
+        <v>58.19751285488933</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -547,10 +547,10 @@
         <v>1000</v>
       </c>
       <c r="E7">
-        <v>1016.698409886167</v>
+        <v>1131.313681695051</v>
       </c>
       <c r="F7">
-        <v>1.669840988616733</v>
+        <v>13.1313681695051</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -567,10 +567,10 @@
         <v>1000</v>
       </c>
       <c r="E8">
-        <v>1024.494620930697</v>
+        <v>1201.301932397386</v>
       </c>
       <c r="F8">
-        <v>2.449462093069699</v>
+        <v>20.13019323973865</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -587,10 +587,10 @@
         <v>1000</v>
       </c>
       <c r="E9">
-        <v>991.3163165158546</v>
+        <v>871.0541417570648</v>
       </c>
       <c r="F9">
-        <v>-0.8683683484145388</v>
+        <v>-12.89458582429351</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -607,10 +607,10 @@
         <v>1000</v>
       </c>
       <c r="E10">
-        <v>991.3163165158546</v>
+        <v>1058.680559134461</v>
       </c>
       <c r="F10">
-        <v>-0.8683683484145388</v>
+        <v>5.868055913446113</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -624,10 +624,10 @@
         <v>1000</v>
       </c>
       <c r="E11">
-        <v>1124.453764535177</v>
+        <v>1144.929498612026</v>
       </c>
       <c r="F11">
-        <v>12.4453764535177</v>
+        <v>14.49294986120265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing a lot of code errors after the course of LSTM. No improvmenet sin results though. Usually alll the predictions are 0 or 1
</commit_message>
<xml_diff>
--- a/backtest_results.xlsx
+++ b/backtest_results.xlsx
@@ -34,10 +34,10 @@
     <t>Cumulative Returns (%)</t>
   </si>
   <si>
-    <t>TSLA</t>
-  </si>
-  <si>
-    <t>AAPL</t>
+    <t>NFE</t>
+  </si>
+  <si>
+    <t>PLUG</t>
   </si>
   <si>
     <t>Ensemble</t>
@@ -450,10 +450,10 @@
         <v>1000</v>
       </c>
       <c r="E2">
-        <v>1306.472775194389</v>
+        <v>-17.14741545364173</v>
       </c>
       <c r="F2">
-        <v>30.64727751943894</v>
+        <v>-101.7147415453642</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -470,10 +470,10 @@
         <v>1000</v>
       </c>
       <c r="E3">
-        <v>773.9697588173583</v>
+        <v>-112.538466017716</v>
       </c>
       <c r="F3">
-        <v>-22.60302411826417</v>
+        <v>-111.2538466017716</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -490,10 +490,10 @@
         <v>1000</v>
       </c>
       <c r="E4">
-        <v>-2029.447346335359</v>
+        <v>1000</v>
       </c>
       <c r="F4">
-        <v>-302.9447346335359</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -510,10 +510,10 @@
         <v>1000</v>
       </c>
       <c r="E5">
-        <v>1581.975128548893</v>
+        <v>49.39116001017241</v>
       </c>
       <c r="F5">
-        <v>58.19751285488933</v>
+        <v>-95.06088399898276</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -527,10 +527,10 @@
         <v>1000</v>
       </c>
       <c r="E6">
-        <v>1000.570825680124</v>
+        <v>610.707381687405</v>
       </c>
       <c r="F6">
-        <v>0.05708256801236758</v>
+        <v>-38.9292618312595</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -547,10 +547,10 @@
         <v>1000</v>
       </c>
       <c r="E7">
-        <v>1131.313681695051</v>
+        <v>414.7290100177484</v>
       </c>
       <c r="F7">
-        <v>13.1313681695051</v>
+        <v>-58.52709899822516</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -567,10 +567,10 @@
         <v>1000</v>
       </c>
       <c r="E8">
-        <v>1201.301932397386</v>
+        <v>685.6608408487546</v>
       </c>
       <c r="F8">
-        <v>20.13019323973865</v>
+        <v>-31.43391591512454</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -587,10 +587,10 @@
         <v>1000</v>
       </c>
       <c r="E9">
-        <v>871.0541417570648</v>
+        <v>1000</v>
       </c>
       <c r="F9">
-        <v>-12.89458582429351</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -607,10 +607,10 @@
         <v>1000</v>
       </c>
       <c r="E10">
-        <v>1058.680559134461</v>
+        <v>391.4648580423796</v>
       </c>
       <c r="F10">
-        <v>5.868055913446113</v>
+        <v>-60.85351419576204</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -624,10 +624,10 @@
         <v>1000</v>
       </c>
       <c r="E11">
-        <v>1144.929498612026</v>
+        <v>385.2095983192128</v>
       </c>
       <c r="F11">
-        <v>14.49294986120265</v>
+        <v>-61.47904016807873</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Skinnied the RF_algo_backtest and Test_train data and added early stopping
</commit_message>
<xml_diff>
--- a/backtest_results.xlsx
+++ b/backtest_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>Stock Ticker</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Cumulative Returns (%)</t>
+  </si>
+  <si>
+    <t>Total Buy Signals</t>
   </si>
   <si>
     <t>NFE</t>
@@ -410,13 +413,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,56 +438,65 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>1000</v>
       </c>
       <c r="E2">
-        <v>-17.14741545364173</v>
+        <v>-168.3878771182665</v>
       </c>
       <c r="F2">
-        <v>-101.7147415453642</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>-116.8387877118267</v>
+      </c>
+      <c r="G2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <v>239.1518985677852</v>
+      </c>
+      <c r="F3">
+        <v>-76.08481014322149</v>
+      </c>
+      <c r="G3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>1000</v>
-      </c>
-      <c r="E3">
-        <v>-112.538466017716</v>
-      </c>
-      <c r="F3">
-        <v>-111.2538466017716</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>1000</v>
@@ -495,33 +507,39 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>1000</v>
       </c>
       <c r="E5">
-        <v>49.39116001017241</v>
+        <v>467.5304207126891</v>
       </c>
       <c r="F5">
-        <v>-95.06088399898276</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>-53.24695792873109</v>
+      </c>
+      <c r="G5">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>1000</v>
@@ -532,56 +550,65 @@
       <c r="F6">
         <v>-38.9292618312595</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>1000</v>
+      </c>
+      <c r="E7">
+        <v>697.2485238905774</v>
+      </c>
+      <c r="F7">
+        <v>-30.27514761094226</v>
+      </c>
+      <c r="G7">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>1000</v>
-      </c>
-      <c r="E7">
-        <v>414.7290100177484</v>
-      </c>
-      <c r="F7">
-        <v>-58.52709899822516</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
       <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>1000</v>
+      </c>
+      <c r="E8">
+        <v>697.2485238905774</v>
+      </c>
+      <c r="F8">
+        <v>-30.27514761094226</v>
+      </c>
+      <c r="G8">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>1000</v>
-      </c>
-      <c r="E8">
-        <v>685.6608408487546</v>
-      </c>
-      <c r="F8">
-        <v>-31.43391591512454</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <v>1000</v>
@@ -592,42 +619,51 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>1000</v>
       </c>
       <c r="E10">
-        <v>391.4648580423796</v>
+        <v>1313.491649519817</v>
       </c>
       <c r="F10">
-        <v>-60.85351419576204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>31.34916495198169</v>
+      </c>
+      <c r="G10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11">
         <v>1000</v>
       </c>
       <c r="E11">
-        <v>385.2095983192128</v>
+        <v>389.1936620642327</v>
       </c>
       <c r="F11">
-        <v>-61.47904016807873</v>
+        <v>-61.08063379357672</v>
+      </c>
+      <c r="G11">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>